<commit_message>
updates code and data
</commit_message>
<xml_diff>
--- a/data/lci_LIB_raw_materials.xlsx
+++ b/data/lci_LIB_raw_materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leidenuniv1-my.sharepoint.com/personal/istrateir_vuw_leidenuniv_nl/Documents/Research/decarbonization_LIB_raw_materials/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2602" documentId="13_ncr:1_{0CD9267C-230F-4C32-BDB0-E201BD3784C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F23B0D02-00B2-42BF-9864-3628D96D4F15}"/>
+  <xr:revisionPtr revIDLastSave="2903" documentId="13_ncr:1_{0CD9267C-230F-4C32-BDB0-E201BD3784C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90DFEBB8-AE69-4174-A794-266558DC12D6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="3" r:id="rId1"/>
@@ -2790,7 +2790,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3035,6 +3035,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3467,10 +3469,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="100" t="s">
         <v>816</v>
       </c>
       <c r="C8" s="31" t="s">
@@ -3481,8 +3483,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="98"/>
-      <c r="B9" s="98"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="100"/>
       <c r="C9" s="31" t="s">
         <v>105</v>
       </c>
@@ -3519,10 +3521,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="98" t="s">
+      <c r="A12" s="100" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="100" t="s">
         <v>482</v>
       </c>
       <c r="C12" s="31" t="s">
@@ -3533,8 +3535,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="98"/>
-      <c r="B13" s="98"/>
+      <c r="A13" s="100"/>
+      <c r="B13" s="100"/>
       <c r="C13" s="50" t="s">
         <v>481</v>
       </c>
@@ -4374,11 +4376,11 @@
       <c r="B7" t="s">
         <v>226</v>
       </c>
-      <c r="C7" s="110">
+      <c r="C7" s="112">
         <f>'Lithium - Spodumene'!D10*'Lithium - Spodumene'!D56/3.6</f>
         <v>0.16610191762962964</v>
       </c>
-      <c r="D7" s="110"/>
+      <c r="D7" s="112"/>
       <c r="E7" s="19">
         <f>'Lithium - Spodumene'!D11</f>
         <v>3.5</v>
@@ -37765,8 +37767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3D24D4-2E6F-41D5-89DB-3F789653CF27}">
   <dimension ref="A1:S87"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42222,16 +42224,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B0F318-8C53-4B11-8704-083389C4343A}">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.28515625" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -43468,6 +43471,36 @@
         <f>Intro!$B$4</f>
         <v>ecoinvent-3.10-cutoff</v>
       </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="59"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="59"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C83" s="37"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C87" s="59"/>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C89" s="99"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="98"/>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="97"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43545,10 +43578,10 @@
       <c r="K5" s="62"/>
     </row>
     <row r="6" spans="1:11" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="101" t="s">
         <v>221</v>
       </c>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="103" t="s">
         <v>699</v>
       </c>
       <c r="C6" s="70" t="s">
@@ -43574,8 +43607,8 @@
       <c r="K6" s="62"/>
     </row>
     <row r="7" spans="1:11" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
+      <c r="A7" s="102"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="66" t="s">
         <v>705</v>
       </c>
@@ -43599,10 +43632,10 @@
       <c r="K7" s="62"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="106" t="s">
         <v>229</v>
       </c>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="103" t="s">
         <v>699</v>
       </c>
       <c r="C8" s="70" t="s">
@@ -43625,8 +43658,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="105"/>
-      <c r="B9" s="101"/>
+      <c r="A9" s="107"/>
+      <c r="B9" s="103"/>
       <c r="C9" s="66" t="s">
         <v>705</v>
       </c>
@@ -43647,8 +43680,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="105"/>
-      <c r="B10" s="101" t="s">
+      <c r="A10" s="107"/>
+      <c r="B10" s="103" t="s">
         <v>702</v>
       </c>
       <c r="C10" s="70" t="s">
@@ -43671,8 +43704,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="105"/>
-      <c r="B11" s="101"/>
+      <c r="A11" s="107"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="66" t="s">
         <v>705</v>
       </c>
@@ -43693,8 +43726,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="105"/>
-      <c r="B12" s="101" t="s">
+      <c r="A12" s="107"/>
+      <c r="B12" s="103" t="s">
         <v>194</v>
       </c>
       <c r="C12" s="70" t="s">
@@ -43717,8 +43750,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="106"/>
-      <c r="B13" s="101"/>
+      <c r="A13" s="108"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="66" t="s">
         <v>705</v>
       </c>
@@ -43739,10 +43772,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="104" t="s">
+      <c r="A14" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="104" t="s">
         <v>472</v>
       </c>
       <c r="C14" s="70" t="s">
@@ -43765,8 +43798,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A15" s="105"/>
-      <c r="B15" s="103"/>
+      <c r="A15" s="107"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="66" t="s">
         <v>705</v>
       </c>
@@ -43787,8 +43820,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="105"/>
-      <c r="B16" s="108" t="s">
+      <c r="A16" s="107"/>
+      <c r="B16" s="110" t="s">
         <v>474</v>
       </c>
       <c r="C16" s="70" t="s">
@@ -43811,8 +43844,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A17" s="105"/>
-      <c r="B17" s="109"/>
+      <c r="A17" s="107"/>
+      <c r="B17" s="111"/>
       <c r="C17" s="66" t="s">
         <v>705</v>
       </c>
@@ -43833,8 +43866,8 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="105"/>
-      <c r="B18" s="108" t="s">
+      <c r="A18" s="107"/>
+      <c r="B18" s="110" t="s">
         <v>475</v>
       </c>
       <c r="C18" s="70" t="s">
@@ -43857,8 +43890,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="106"/>
-      <c r="B19" s="109"/>
+      <c r="A19" s="108"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="66" t="s">
         <v>705</v>
       </c>
@@ -43880,10 +43913,10 @@
       <c r="K19" s="77"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="104" t="s">
+      <c r="A20" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="108" t="s">
+      <c r="B20" s="110" t="s">
         <v>726</v>
       </c>
       <c r="C20" s="70" t="s">
@@ -43907,8 +43940,8 @@
       <c r="K20" s="77"/>
     </row>
     <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="106"/>
-      <c r="B21" s="109"/>
+      <c r="A21" s="108"/>
+      <c r="B21" s="111"/>
       <c r="C21" s="66" t="s">
         <v>705</v>
       </c>
@@ -43930,10 +43963,10 @@
       <c r="K21" s="77"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="107" t="s">
+      <c r="A22" s="109" t="s">
         <v>725</v>
       </c>
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="104" t="s">
         <v>515</v>
       </c>
       <c r="C22" s="70" t="s">
@@ -43956,8 +43989,8 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
-      <c r="B23" s="103"/>
+      <c r="A23" s="109"/>
+      <c r="B23" s="105"/>
       <c r="C23" s="66" t="s">
         <v>705</v>
       </c>
@@ -43979,8 +44012,8 @@
       <c r="K23" s="74"/>
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="107"/>
-      <c r="B24" s="102" t="s">
+      <c r="A24" s="109"/>
+      <c r="B24" s="104" t="s">
         <v>487</v>
       </c>
       <c r="C24" s="70" t="s">
@@ -44003,8 +44036,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="107"/>
-      <c r="B25" s="103"/>
+      <c r="A25" s="109"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="66" t="s">
         <v>705</v>
       </c>
@@ -44025,8 +44058,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="107"/>
-      <c r="B26" s="101" t="s">
+      <c r="A26" s="109"/>
+      <c r="B26" s="103" t="s">
         <v>524</v>
       </c>
       <c r="C26" s="70" t="s">
@@ -44049,8 +44082,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A27" s="107"/>
-      <c r="B27" s="101"/>
+      <c r="A27" s="109"/>
+      <c r="B27" s="103"/>
       <c r="C27" s="66" t="s">
         <v>705</v>
       </c>
@@ -44071,8 +44104,8 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="107"/>
-      <c r="B28" s="101" t="s">
+      <c r="A28" s="109"/>
+      <c r="B28" s="103" t="s">
         <v>490</v>
       </c>
       <c r="C28" s="70" t="s">
@@ -44095,8 +44128,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="107"/>
-      <c r="B29" s="101"/>
+      <c r="A29" s="109"/>
+      <c r="B29" s="103"/>
       <c r="C29" s="66" t="s">
         <v>705</v>
       </c>
@@ -44117,8 +44150,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="107"/>
-      <c r="B30" s="101" t="s">
+      <c r="A30" s="109"/>
+      <c r="B30" s="103" t="s">
         <v>491</v>
       </c>
       <c r="C30" s="70" t="s">
@@ -44141,8 +44174,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
-      <c r="B31" s="101"/>
+      <c r="A31" s="109"/>
+      <c r="B31" s="103"/>
       <c r="C31" s="66" t="s">
         <v>705</v>
       </c>
@@ -44163,8 +44196,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="107"/>
-      <c r="B32" s="101" t="s">
+      <c r="A32" s="109"/>
+      <c r="B32" s="103" t="s">
         <v>494</v>
       </c>
       <c r="C32" s="70" t="s">
@@ -44187,8 +44220,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
-      <c r="B33" s="101"/>
+      <c r="A33" s="109"/>
+      <c r="B33" s="103"/>
       <c r="C33" s="66" t="s">
         <v>705</v>
       </c>

</xml_diff>